<commit_message>
Everything now is working correctly!!
</commit_message>
<xml_diff>
--- a/QUML_Keystrokes/MD_Double_Check.xlsx
+++ b/QUML_Keystrokes/MD_Double_Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="User 1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="User 3" sheetId="3" r:id="rId3"/>
     <sheet name="User 4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -353,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,6 +589,126 @@
       </c>
       <c r="G10">
         <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>175.1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>171.9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>234.3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>479.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>356.1</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>200.1</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>201.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f>ABS(A1-A12)/10</f>
+        <v>1.9099999999999995</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:G14" si="1">ABS(B1-B12)/10</f>
+        <v>1.6099999999999994</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>3.169999999999999</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>10.48</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1.3100000000000023</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>1.8900000000000006</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000057</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f>ABS(A2-A12)/10</f>
+        <v>0.30999999999999944</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:G15" si="2">ABS(B2-B12)/10</f>
+        <v>6.31</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>7.7699999999999987</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0.2899999999999977</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>0.29000000000000059</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>3.3400000000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>ABS(A3-A12)/10</f>
+        <v>1.8099999999999994</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:G16" si="3">ABS(B3-B12)/10</f>
+        <v>1.5099999999999993</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>3.169999999999999</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>16.78</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>1.2100000000000022</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>1.2099999999999995</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>1.6400000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -1088,10 +1208,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1326,6 +1446,36 @@
         <v>188</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>215.5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>215.6</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>293.7</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>612.5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>396.9</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>231.3</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>176.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
MOre data being added, and more code being written.
</commit_message>
<xml_diff>
--- a/QUML_Keystrokes/MD_Double_Check.xlsx
+++ b/QUML_Keystrokes/MD_Double_Check.xlsx
@@ -4,13 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="User 1" sheetId="1" r:id="rId1"/>
     <sheet name="User 2" sheetId="2" r:id="rId2"/>
     <sheet name="User 3" sheetId="3" r:id="rId3"/>
     <sheet name="User 4" sheetId="4" r:id="rId4"/>
+    <sheet name="User 5" sheetId="5" r:id="rId5"/>
+    <sheet name="User 6" sheetId="6" r:id="rId6"/>
+    <sheet name="User 7" sheetId="7" r:id="rId7"/>
+    <sheet name="User 8" sheetId="8" r:id="rId8"/>
+    <sheet name="User 9" sheetId="9" r:id="rId9"/>
+    <sheet name="User 10" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
@@ -355,8 +361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,244 +722,274 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>187</v>
+        <v>125</v>
       </c>
       <c r="B1">
-        <v>188</v>
+        <v>110</v>
       </c>
       <c r="C1">
-        <v>250</v>
+        <v>328</v>
       </c>
       <c r="D1">
-        <v>547</v>
+        <v>281</v>
       </c>
       <c r="E1">
-        <v>406</v>
+        <v>375</v>
       </c>
       <c r="F1">
-        <v>234</v>
+        <v>375</v>
       </c>
       <c r="G1">
-        <v>313</v>
+        <v>156</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>234</v>
+        <v>125</v>
       </c>
       <c r="B2">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="C2">
-        <v>187</v>
+        <v>235</v>
       </c>
       <c r="D2">
-        <v>344</v>
+        <v>500</v>
       </c>
       <c r="E2">
-        <v>391</v>
+        <v>359</v>
       </c>
       <c r="F2">
-        <v>234</v>
+        <v>375</v>
       </c>
       <c r="G2">
-        <v>281</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>188</v>
+        <v>156</v>
       </c>
       <c r="B3">
         <v>172</v>
       </c>
       <c r="C3">
-        <v>187</v>
+        <v>328</v>
       </c>
       <c r="D3">
         <v>297</v>
       </c>
       <c r="E3">
-        <v>313</v>
+        <v>406</v>
       </c>
       <c r="F3">
-        <v>515</v>
+        <v>297</v>
       </c>
       <c r="G3">
-        <v>157</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
+        <v>125</v>
+      </c>
+      <c r="B4">
         <v>156</v>
       </c>
-      <c r="B4">
-        <v>172</v>
-      </c>
       <c r="C4">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="D4">
-        <v>375</v>
+        <v>391</v>
       </c>
       <c r="E4">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="F4">
         <v>282</v>
       </c>
       <c r="G4">
-        <v>312</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>140</v>
+        <v>93</v>
       </c>
       <c r="B5">
-        <v>188</v>
+        <v>141</v>
       </c>
       <c r="C5">
-        <v>312</v>
+        <v>281</v>
       </c>
       <c r="D5">
         <v>344</v>
       </c>
       <c r="E5">
-        <v>281</v>
+        <v>359</v>
       </c>
       <c r="F5">
-        <v>266</v>
+        <v>313</v>
       </c>
       <c r="G5">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="B6">
-        <v>375</v>
+        <v>140</v>
       </c>
       <c r="C6">
-        <v>281</v>
+        <v>188</v>
       </c>
       <c r="D6">
-        <v>266</v>
+        <v>312</v>
       </c>
       <c r="E6">
         <v>328</v>
       </c>
       <c r="F6">
-        <v>312</v>
+        <v>250</v>
       </c>
       <c r="G6">
-        <v>250</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="B7">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="C7">
-        <v>250</v>
+        <v>188</v>
       </c>
       <c r="D7">
-        <v>438</v>
+        <v>343</v>
       </c>
       <c r="E7">
-        <v>437</v>
+        <v>469</v>
       </c>
       <c r="F7">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="G7">
-        <v>235</v>
+        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="B8">
-        <v>187</v>
+        <v>109</v>
       </c>
       <c r="C8">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="D8">
-        <v>281</v>
+        <v>453</v>
       </c>
       <c r="E8">
-        <v>328</v>
+        <v>391</v>
       </c>
       <c r="F8">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G8">
-        <v>203</v>
+        <v>282</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>172</v>
+        <v>94</v>
       </c>
       <c r="B9">
-        <v>172</v>
+        <v>140</v>
       </c>
       <c r="C9">
-        <v>188</v>
+        <v>235</v>
       </c>
       <c r="D9">
         <v>281</v>
       </c>
       <c r="E9">
-        <v>328</v>
+        <v>359</v>
       </c>
       <c r="F9">
-        <v>297</v>
+        <v>235</v>
       </c>
       <c r="G9">
-        <v>234</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10">
+        <v>125</v>
+      </c>
+      <c r="C10">
+        <v>359</v>
+      </c>
+      <c r="D10">
+        <v>297</v>
+      </c>
+      <c r="E10">
+        <v>266</v>
+      </c>
+      <c r="F10">
+        <v>265</v>
+      </c>
+      <c r="G10">
         <v>141</v>
       </c>
-      <c r="B10">
-        <v>156</v>
-      </c>
-      <c r="C10">
-        <v>188</v>
-      </c>
-      <c r="D10">
-        <v>375</v>
-      </c>
-      <c r="E10">
-        <v>312</v>
-      </c>
-      <c r="F10">
-        <v>281</v>
-      </c>
-      <c r="G10">
-        <v>219</v>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>123.5</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>140.5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>248.6</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>349.9</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>362.4</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>304.7</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -961,252 +997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>235</v>
-      </c>
-      <c r="B1">
-        <v>265</v>
-      </c>
-      <c r="C1">
-        <v>1235</v>
-      </c>
-      <c r="D1">
-        <v>531</v>
-      </c>
-      <c r="E1">
-        <v>453</v>
-      </c>
-      <c r="F1">
-        <v>406</v>
-      </c>
-      <c r="G1">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>235</v>
-      </c>
-      <c r="B2">
-        <v>265</v>
-      </c>
-      <c r="C2">
-        <v>1235</v>
-      </c>
-      <c r="D2">
-        <v>531</v>
-      </c>
-      <c r="E2">
-        <v>453</v>
-      </c>
-      <c r="F2">
-        <v>406</v>
-      </c>
-      <c r="G2">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>235</v>
-      </c>
-      <c r="B3">
-        <v>265</v>
-      </c>
-      <c r="C3">
-        <v>1235</v>
-      </c>
-      <c r="D3">
-        <v>531</v>
-      </c>
-      <c r="E3">
-        <v>453</v>
-      </c>
-      <c r="F3">
-        <v>406</v>
-      </c>
-      <c r="G3">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>235</v>
-      </c>
-      <c r="B4">
-        <v>265</v>
-      </c>
-      <c r="C4">
-        <v>1235</v>
-      </c>
-      <c r="D4">
-        <v>531</v>
-      </c>
-      <c r="E4">
-        <v>453</v>
-      </c>
-      <c r="F4">
-        <v>406</v>
-      </c>
-      <c r="G4">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>344</v>
-      </c>
-      <c r="B5">
-        <v>312</v>
-      </c>
-      <c r="C5">
-        <v>954</v>
-      </c>
-      <c r="D5">
-        <v>640</v>
-      </c>
-      <c r="E5">
-        <v>469</v>
-      </c>
-      <c r="F5">
-        <v>375</v>
-      </c>
-      <c r="G5">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>312</v>
-      </c>
-      <c r="B6">
-        <v>313</v>
-      </c>
-      <c r="C6">
-        <v>1156</v>
-      </c>
-      <c r="D6">
-        <v>500</v>
-      </c>
-      <c r="E6">
-        <v>453</v>
-      </c>
-      <c r="F6">
-        <v>359</v>
-      </c>
-      <c r="G6">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>265</v>
-      </c>
-      <c r="B7">
-        <v>281</v>
-      </c>
-      <c r="C7">
-        <v>1313</v>
-      </c>
-      <c r="D7">
-        <v>562</v>
-      </c>
-      <c r="E7">
-        <v>500</v>
-      </c>
-      <c r="F7">
-        <v>313</v>
-      </c>
-      <c r="G7">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>297</v>
-      </c>
-      <c r="B8">
-        <v>266</v>
-      </c>
-      <c r="C8">
-        <v>1406</v>
-      </c>
-      <c r="D8">
-        <v>391</v>
-      </c>
-      <c r="E8">
-        <v>453</v>
-      </c>
-      <c r="F8">
-        <v>406</v>
-      </c>
-      <c r="G8">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>328</v>
-      </c>
-      <c r="B9">
-        <v>375</v>
-      </c>
-      <c r="C9">
-        <v>813</v>
-      </c>
-      <c r="D9">
-        <v>547</v>
-      </c>
-      <c r="E9">
-        <v>547</v>
-      </c>
-      <c r="F9">
-        <v>343</v>
-      </c>
-      <c r="G9">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>250</v>
-      </c>
-      <c r="B10">
-        <v>312</v>
-      </c>
-      <c r="C10">
-        <v>609</v>
-      </c>
-      <c r="D10">
-        <v>469</v>
-      </c>
-      <c r="E10">
-        <v>688</v>
-      </c>
-      <c r="F10">
-        <v>359</v>
-      </c>
-      <c r="G10">
-        <v>344</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
@@ -1218,6 +1009,556 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
+        <v>187</v>
+      </c>
+      <c r="B1">
+        <v>188</v>
+      </c>
+      <c r="C1">
+        <v>250</v>
+      </c>
+      <c r="D1">
+        <v>547</v>
+      </c>
+      <c r="E1">
+        <v>406</v>
+      </c>
+      <c r="F1">
+        <v>234</v>
+      </c>
+      <c r="G1">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>234</v>
+      </c>
+      <c r="B2">
+        <v>188</v>
+      </c>
+      <c r="C2">
+        <v>187</v>
+      </c>
+      <c r="D2">
+        <v>344</v>
+      </c>
+      <c r="E2">
+        <v>391</v>
+      </c>
+      <c r="F2">
+        <v>234</v>
+      </c>
+      <c r="G2">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>188</v>
+      </c>
+      <c r="B3">
+        <v>172</v>
+      </c>
+      <c r="C3">
+        <v>187</v>
+      </c>
+      <c r="D3">
+        <v>297</v>
+      </c>
+      <c r="E3">
+        <v>313</v>
+      </c>
+      <c r="F3">
+        <v>515</v>
+      </c>
+      <c r="G3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>156</v>
+      </c>
+      <c r="B4">
+        <v>172</v>
+      </c>
+      <c r="C4">
+        <v>203</v>
+      </c>
+      <c r="D4">
+        <v>375</v>
+      </c>
+      <c r="E4">
+        <v>328</v>
+      </c>
+      <c r="F4">
+        <v>282</v>
+      </c>
+      <c r="G4">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>140</v>
+      </c>
+      <c r="B5">
+        <v>188</v>
+      </c>
+      <c r="C5">
+        <v>312</v>
+      </c>
+      <c r="D5">
+        <v>344</v>
+      </c>
+      <c r="E5">
+        <v>281</v>
+      </c>
+      <c r="F5">
+        <v>266</v>
+      </c>
+      <c r="G5">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>156</v>
+      </c>
+      <c r="B6">
+        <v>375</v>
+      </c>
+      <c r="C6">
+        <v>281</v>
+      </c>
+      <c r="D6">
+        <v>266</v>
+      </c>
+      <c r="E6">
+        <v>328</v>
+      </c>
+      <c r="F6">
+        <v>312</v>
+      </c>
+      <c r="G6">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>141</v>
+      </c>
+      <c r="B7">
+        <v>187</v>
+      </c>
+      <c r="C7">
+        <v>250</v>
+      </c>
+      <c r="D7">
+        <v>438</v>
+      </c>
+      <c r="E7">
+        <v>437</v>
+      </c>
+      <c r="F7">
+        <v>328</v>
+      </c>
+      <c r="G7">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>157</v>
+      </c>
+      <c r="B8">
+        <v>187</v>
+      </c>
+      <c r="C8">
+        <v>188</v>
+      </c>
+      <c r="D8">
+        <v>281</v>
+      </c>
+      <c r="E8">
+        <v>328</v>
+      </c>
+      <c r="F8">
+        <v>297</v>
+      </c>
+      <c r="G8">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>172</v>
+      </c>
+      <c r="B9">
+        <v>172</v>
+      </c>
+      <c r="C9">
+        <v>188</v>
+      </c>
+      <c r="D9">
+        <v>281</v>
+      </c>
+      <c r="E9">
+        <v>328</v>
+      </c>
+      <c r="F9">
+        <v>297</v>
+      </c>
+      <c r="G9">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>141</v>
+      </c>
+      <c r="B10">
+        <v>156</v>
+      </c>
+      <c r="C10">
+        <v>188</v>
+      </c>
+      <c r="D10">
+        <v>375</v>
+      </c>
+      <c r="E10">
+        <v>312</v>
+      </c>
+      <c r="F10">
+        <v>281</v>
+      </c>
+      <c r="G10">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>167.2</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>198.5</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>223.4</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>354.8</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>345.2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>304.60000000000002</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>242.3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>235</v>
+      </c>
+      <c r="B1">
+        <v>265</v>
+      </c>
+      <c r="C1">
+        <v>1235</v>
+      </c>
+      <c r="D1">
+        <v>531</v>
+      </c>
+      <c r="E1">
+        <v>453</v>
+      </c>
+      <c r="F1">
+        <v>406</v>
+      </c>
+      <c r="G1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>235</v>
+      </c>
+      <c r="B2">
+        <v>265</v>
+      </c>
+      <c r="C2">
+        <v>1235</v>
+      </c>
+      <c r="D2">
+        <v>531</v>
+      </c>
+      <c r="E2">
+        <v>453</v>
+      </c>
+      <c r="F2">
+        <v>406</v>
+      </c>
+      <c r="G2">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>235</v>
+      </c>
+      <c r="B3">
+        <v>265</v>
+      </c>
+      <c r="C3">
+        <v>1235</v>
+      </c>
+      <c r="D3">
+        <v>531</v>
+      </c>
+      <c r="E3">
+        <v>453</v>
+      </c>
+      <c r="F3">
+        <v>406</v>
+      </c>
+      <c r="G3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>235</v>
+      </c>
+      <c r="B4">
+        <v>265</v>
+      </c>
+      <c r="C4">
+        <v>1235</v>
+      </c>
+      <c r="D4">
+        <v>531</v>
+      </c>
+      <c r="E4">
+        <v>453</v>
+      </c>
+      <c r="F4">
+        <v>406</v>
+      </c>
+      <c r="G4">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>344</v>
+      </c>
+      <c r="B5">
+        <v>312</v>
+      </c>
+      <c r="C5">
+        <v>954</v>
+      </c>
+      <c r="D5">
+        <v>640</v>
+      </c>
+      <c r="E5">
+        <v>469</v>
+      </c>
+      <c r="F5">
+        <v>375</v>
+      </c>
+      <c r="G5">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>312</v>
+      </c>
+      <c r="B6">
+        <v>313</v>
+      </c>
+      <c r="C6">
+        <v>1156</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6">
+        <v>453</v>
+      </c>
+      <c r="F6">
+        <v>359</v>
+      </c>
+      <c r="G6">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>265</v>
+      </c>
+      <c r="B7">
+        <v>281</v>
+      </c>
+      <c r="C7">
+        <v>1313</v>
+      </c>
+      <c r="D7">
+        <v>562</v>
+      </c>
+      <c r="E7">
+        <v>500</v>
+      </c>
+      <c r="F7">
+        <v>313</v>
+      </c>
+      <c r="G7">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>297</v>
+      </c>
+      <c r="B8">
+        <v>266</v>
+      </c>
+      <c r="C8">
+        <v>1406</v>
+      </c>
+      <c r="D8">
+        <v>391</v>
+      </c>
+      <c r="E8">
+        <v>453</v>
+      </c>
+      <c r="F8">
+        <v>406</v>
+      </c>
+      <c r="G8">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>328</v>
+      </c>
+      <c r="B9">
+        <v>375</v>
+      </c>
+      <c r="C9">
+        <v>813</v>
+      </c>
+      <c r="D9">
+        <v>547</v>
+      </c>
+      <c r="E9">
+        <v>547</v>
+      </c>
+      <c r="F9">
+        <v>343</v>
+      </c>
+      <c r="G9">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>250</v>
+      </c>
+      <c r="B10">
+        <v>312</v>
+      </c>
+      <c r="C10">
+        <v>609</v>
+      </c>
+      <c r="D10">
+        <v>469</v>
+      </c>
+      <c r="E10">
+        <v>688</v>
+      </c>
+      <c r="F10">
+        <v>359</v>
+      </c>
+      <c r="G10">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>273.60000000000002</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>291.89999999999998</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>1119.0999999999999</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>523.29999999999995</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>492.2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>377.9</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>317.60000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
         <v>172</v>
       </c>
       <c r="B1">
@@ -1479,4 +1820,1372 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>204</v>
+      </c>
+      <c r="B1">
+        <v>218</v>
+      </c>
+      <c r="C1">
+        <v>641</v>
+      </c>
+      <c r="D1">
+        <v>656</v>
+      </c>
+      <c r="E1">
+        <v>500</v>
+      </c>
+      <c r="F1">
+        <v>235</v>
+      </c>
+      <c r="G1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>219</v>
+      </c>
+      <c r="B2">
+        <v>203</v>
+      </c>
+      <c r="C2">
+        <v>657</v>
+      </c>
+      <c r="D2">
+        <v>593</v>
+      </c>
+      <c r="E2">
+        <v>578</v>
+      </c>
+      <c r="F2">
+        <v>219</v>
+      </c>
+      <c r="G2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>219</v>
+      </c>
+      <c r="B3">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>328</v>
+      </c>
+      <c r="D3">
+        <v>812</v>
+      </c>
+      <c r="E3">
+        <v>547</v>
+      </c>
+      <c r="F3">
+        <v>235</v>
+      </c>
+      <c r="G3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>188</v>
+      </c>
+      <c r="B4">
+        <v>250</v>
+      </c>
+      <c r="C4">
+        <v>578</v>
+      </c>
+      <c r="D4">
+        <v>328</v>
+      </c>
+      <c r="E4">
+        <v>344</v>
+      </c>
+      <c r="F4">
+        <v>297</v>
+      </c>
+      <c r="G4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>375</v>
+      </c>
+      <c r="B5">
+        <v>281</v>
+      </c>
+      <c r="C5">
+        <v>329</v>
+      </c>
+      <c r="D5">
+        <v>437</v>
+      </c>
+      <c r="E5">
+        <v>578</v>
+      </c>
+      <c r="F5">
+        <v>250</v>
+      </c>
+      <c r="G5">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>188</v>
+      </c>
+      <c r="B6">
+        <v>265</v>
+      </c>
+      <c r="C6">
+        <v>891</v>
+      </c>
+      <c r="D6">
+        <v>484</v>
+      </c>
+      <c r="E6">
+        <v>594</v>
+      </c>
+      <c r="F6">
+        <v>266</v>
+      </c>
+      <c r="G6">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>313</v>
+      </c>
+      <c r="B7">
+        <v>312</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>375</v>
+      </c>
+      <c r="E7">
+        <v>547</v>
+      </c>
+      <c r="F7">
+        <v>250</v>
+      </c>
+      <c r="G7">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>188</v>
+      </c>
+      <c r="B8">
+        <v>250</v>
+      </c>
+      <c r="C8">
+        <v>281</v>
+      </c>
+      <c r="D8">
+        <v>360</v>
+      </c>
+      <c r="E8">
+        <v>390</v>
+      </c>
+      <c r="F8">
+        <v>250</v>
+      </c>
+      <c r="G8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>218</v>
+      </c>
+      <c r="B9">
+        <v>219</v>
+      </c>
+      <c r="C9">
+        <v>578</v>
+      </c>
+      <c r="D9">
+        <v>219</v>
+      </c>
+      <c r="E9">
+        <v>563</v>
+      </c>
+      <c r="F9">
+        <v>250</v>
+      </c>
+      <c r="G9">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>157</v>
+      </c>
+      <c r="B10">
+        <v>234</v>
+      </c>
+      <c r="C10">
+        <v>312</v>
+      </c>
+      <c r="D10">
+        <v>266</v>
+      </c>
+      <c r="E10">
+        <v>344</v>
+      </c>
+      <c r="F10">
+        <v>297</v>
+      </c>
+      <c r="G10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>157</v>
+      </c>
+      <c r="B11">
+        <v>234</v>
+      </c>
+      <c r="C11">
+        <v>312</v>
+      </c>
+      <c r="D11">
+        <v>266</v>
+      </c>
+      <c r="E11">
+        <v>344</v>
+      </c>
+      <c r="F11">
+        <v>297</v>
+      </c>
+      <c r="G11">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>125</v>
+      </c>
+      <c r="B1">
+        <v>187</v>
+      </c>
+      <c r="C1">
+        <v>141</v>
+      </c>
+      <c r="D1">
+        <v>328</v>
+      </c>
+      <c r="E1">
+        <v>672</v>
+      </c>
+      <c r="F1">
+        <v>203</v>
+      </c>
+      <c r="G1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>62</v>
+      </c>
+      <c r="B2">
+        <v>219</v>
+      </c>
+      <c r="C2">
+        <v>94</v>
+      </c>
+      <c r="D2">
+        <v>375</v>
+      </c>
+      <c r="E2">
+        <v>609</v>
+      </c>
+      <c r="F2">
+        <v>63</v>
+      </c>
+      <c r="G2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>63</v>
+      </c>
+      <c r="B3">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>109</v>
+      </c>
+      <c r="D3">
+        <v>391</v>
+      </c>
+      <c r="E3">
+        <v>578</v>
+      </c>
+      <c r="F3">
+        <v>125</v>
+      </c>
+      <c r="G3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>203</v>
+      </c>
+      <c r="C4">
+        <v>125</v>
+      </c>
+      <c r="D4">
+        <v>390</v>
+      </c>
+      <c r="E4">
+        <v>641</v>
+      </c>
+      <c r="F4">
+        <v>62</v>
+      </c>
+      <c r="G4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>47</v>
+      </c>
+      <c r="B5">
+        <v>219</v>
+      </c>
+      <c r="C5">
+        <v>141</v>
+      </c>
+      <c r="D5">
+        <v>687</v>
+      </c>
+      <c r="E5">
+        <v>578</v>
+      </c>
+      <c r="F5">
+        <v>188</v>
+      </c>
+      <c r="G5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>203</v>
+      </c>
+      <c r="C6">
+        <v>172</v>
+      </c>
+      <c r="D6">
+        <v>250</v>
+      </c>
+      <c r="E6">
+        <v>609</v>
+      </c>
+      <c r="F6">
+        <v>78</v>
+      </c>
+      <c r="G6">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>79</v>
+      </c>
+      <c r="B7">
+        <v>203</v>
+      </c>
+      <c r="C7">
+        <v>125</v>
+      </c>
+      <c r="D7">
+        <v>281</v>
+      </c>
+      <c r="E7">
+        <v>703</v>
+      </c>
+      <c r="F7">
+        <v>109</v>
+      </c>
+      <c r="G7">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>47</v>
+      </c>
+      <c r="B8">
+        <v>203</v>
+      </c>
+      <c r="C8">
+        <v>110</v>
+      </c>
+      <c r="D8">
+        <v>328</v>
+      </c>
+      <c r="E8">
+        <v>562</v>
+      </c>
+      <c r="F8">
+        <v>141</v>
+      </c>
+      <c r="G8">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>204</v>
+      </c>
+      <c r="C9">
+        <v>93</v>
+      </c>
+      <c r="D9">
+        <v>375</v>
+      </c>
+      <c r="E9">
+        <v>563</v>
+      </c>
+      <c r="F9">
+        <v>250</v>
+      </c>
+      <c r="G9">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>47</v>
+      </c>
+      <c r="B10">
+        <v>219</v>
+      </c>
+      <c r="C10">
+        <v>93</v>
+      </c>
+      <c r="D10">
+        <v>329</v>
+      </c>
+      <c r="E10">
+        <v>593</v>
+      </c>
+      <c r="F10">
+        <v>157</v>
+      </c>
+      <c r="G10">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>64.2</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>207.9</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>120.3</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>373.4</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>610.79999999999995</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>137.6</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>232.7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>171</v>
+      </c>
+      <c r="B1">
+        <v>172</v>
+      </c>
+      <c r="C1">
+        <v>328</v>
+      </c>
+      <c r="D1">
+        <v>360</v>
+      </c>
+      <c r="E1">
+        <v>281</v>
+      </c>
+      <c r="F1">
+        <v>188</v>
+      </c>
+      <c r="G1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>110</v>
+      </c>
+      <c r="B2">
+        <v>140</v>
+      </c>
+      <c r="C2">
+        <v>313</v>
+      </c>
+      <c r="D2">
+        <v>328</v>
+      </c>
+      <c r="E2">
+        <v>437</v>
+      </c>
+      <c r="F2">
+        <v>266</v>
+      </c>
+      <c r="G2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>141</v>
+      </c>
+      <c r="B3">
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <v>344</v>
+      </c>
+      <c r="D3">
+        <v>375</v>
+      </c>
+      <c r="E3">
+        <v>328</v>
+      </c>
+      <c r="F3">
+        <v>219</v>
+      </c>
+      <c r="G3">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>203</v>
+      </c>
+      <c r="B4">
+        <v>156</v>
+      </c>
+      <c r="C4">
+        <v>422</v>
+      </c>
+      <c r="D4">
+        <v>359</v>
+      </c>
+      <c r="E4">
+        <v>422</v>
+      </c>
+      <c r="F4">
+        <v>172</v>
+      </c>
+      <c r="G4">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>140</v>
+      </c>
+      <c r="B5">
+        <v>156</v>
+      </c>
+      <c r="C5">
+        <v>250</v>
+      </c>
+      <c r="D5">
+        <v>360</v>
+      </c>
+      <c r="E5">
+        <v>328</v>
+      </c>
+      <c r="F5">
+        <v>187</v>
+      </c>
+      <c r="G5">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>140</v>
+      </c>
+      <c r="B6">
+        <v>125</v>
+      </c>
+      <c r="C6">
+        <v>391</v>
+      </c>
+      <c r="D6">
+        <v>344</v>
+      </c>
+      <c r="E6">
+        <v>343</v>
+      </c>
+      <c r="F6">
+        <v>203</v>
+      </c>
+      <c r="G6">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>140</v>
+      </c>
+      <c r="B7">
+        <v>141</v>
+      </c>
+      <c r="C7">
+        <v>281</v>
+      </c>
+      <c r="D7">
+        <v>406</v>
+      </c>
+      <c r="E7">
+        <v>391</v>
+      </c>
+      <c r="F7">
+        <v>203</v>
+      </c>
+      <c r="G7">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>141</v>
+      </c>
+      <c r="B8">
+        <v>109</v>
+      </c>
+      <c r="C8">
+        <v>188</v>
+      </c>
+      <c r="D8">
+        <v>515</v>
+      </c>
+      <c r="E8">
+        <v>313</v>
+      </c>
+      <c r="F8">
+        <v>172</v>
+      </c>
+      <c r="G8">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>141</v>
+      </c>
+      <c r="B9">
+        <v>141</v>
+      </c>
+      <c r="C9">
+        <v>234</v>
+      </c>
+      <c r="D9">
+        <v>328</v>
+      </c>
+      <c r="E9">
+        <v>313</v>
+      </c>
+      <c r="F9">
+        <v>187</v>
+      </c>
+      <c r="G9">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>156</v>
+      </c>
+      <c r="B10">
+        <v>141</v>
+      </c>
+      <c r="C10">
+        <v>219</v>
+      </c>
+      <c r="D10">
+        <v>312</v>
+      </c>
+      <c r="E10">
+        <v>281</v>
+      </c>
+      <c r="F10">
+        <v>172</v>
+      </c>
+      <c r="G10">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>148.30000000000001</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>140.6</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>297</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>368.7</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>343.7</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>196.9</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>182.9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>187</v>
+      </c>
+      <c r="B1">
+        <v>141</v>
+      </c>
+      <c r="C1">
+        <v>234</v>
+      </c>
+      <c r="D1">
+        <v>578</v>
+      </c>
+      <c r="E1">
+        <v>360</v>
+      </c>
+      <c r="F1">
+        <v>609</v>
+      </c>
+      <c r="G1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>156</v>
+      </c>
+      <c r="B2">
+        <v>125</v>
+      </c>
+      <c r="C2">
+        <v>219</v>
+      </c>
+      <c r="D2">
+        <v>781</v>
+      </c>
+      <c r="E2">
+        <v>282</v>
+      </c>
+      <c r="F2">
+        <v>484</v>
+      </c>
+      <c r="G2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>172</v>
+      </c>
+      <c r="B3">
+        <v>125</v>
+      </c>
+      <c r="C3">
+        <v>187</v>
+      </c>
+      <c r="D3">
+        <v>688</v>
+      </c>
+      <c r="E3">
+        <v>281</v>
+      </c>
+      <c r="F3">
+        <v>578</v>
+      </c>
+      <c r="G3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>204</v>
+      </c>
+      <c r="B4">
+        <v>140</v>
+      </c>
+      <c r="C4">
+        <v>219</v>
+      </c>
+      <c r="D4">
+        <v>594</v>
+      </c>
+      <c r="E4">
+        <v>359</v>
+      </c>
+      <c r="F4">
+        <v>609</v>
+      </c>
+      <c r="G4">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>203</v>
+      </c>
+      <c r="B5">
+        <v>125</v>
+      </c>
+      <c r="C5">
+        <v>328</v>
+      </c>
+      <c r="D5">
+        <v>516</v>
+      </c>
+      <c r="E5">
+        <v>297</v>
+      </c>
+      <c r="F5">
+        <v>453</v>
+      </c>
+      <c r="G5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>203</v>
+      </c>
+      <c r="B6">
+        <v>125</v>
+      </c>
+      <c r="C6">
+        <v>328</v>
+      </c>
+      <c r="D6">
+        <v>516</v>
+      </c>
+      <c r="E6">
+        <v>297</v>
+      </c>
+      <c r="F6">
+        <v>453</v>
+      </c>
+      <c r="G6">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>203</v>
+      </c>
+      <c r="B7">
+        <v>125</v>
+      </c>
+      <c r="C7">
+        <v>328</v>
+      </c>
+      <c r="D7">
+        <v>516</v>
+      </c>
+      <c r="E7">
+        <v>297</v>
+      </c>
+      <c r="F7">
+        <v>453</v>
+      </c>
+      <c r="G7">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>375</v>
+      </c>
+      <c r="B8">
+        <v>140</v>
+      </c>
+      <c r="C8">
+        <v>204</v>
+      </c>
+      <c r="D8">
+        <v>312</v>
+      </c>
+      <c r="E8">
+        <v>313</v>
+      </c>
+      <c r="F8">
+        <v>437</v>
+      </c>
+      <c r="G8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>343</v>
+      </c>
+      <c r="B9">
+        <v>110</v>
+      </c>
+      <c r="C9">
+        <v>234</v>
+      </c>
+      <c r="D9">
+        <v>500</v>
+      </c>
+      <c r="E9">
+        <v>313</v>
+      </c>
+      <c r="F9">
+        <v>359</v>
+      </c>
+      <c r="G9">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>203</v>
+      </c>
+      <c r="B10">
+        <v>125</v>
+      </c>
+      <c r="C10">
+        <v>328</v>
+      </c>
+      <c r="D10">
+        <v>516</v>
+      </c>
+      <c r="E10">
+        <v>297</v>
+      </c>
+      <c r="F10">
+        <v>453</v>
+      </c>
+      <c r="G10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>224.9</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>128.1</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>260.89999999999998</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>551.70000000000005</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>309.60000000000002</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>488.8</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>137.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12:G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>63</v>
+      </c>
+      <c r="B1">
+        <v>203</v>
+      </c>
+      <c r="C1">
+        <v>656</v>
+      </c>
+      <c r="D1">
+        <v>422</v>
+      </c>
+      <c r="E1">
+        <v>266</v>
+      </c>
+      <c r="F1">
+        <v>234</v>
+      </c>
+      <c r="G1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>125</v>
+      </c>
+      <c r="B2">
+        <v>203</v>
+      </c>
+      <c r="C2">
+        <v>953</v>
+      </c>
+      <c r="D2">
+        <v>547</v>
+      </c>
+      <c r="E2">
+        <v>375</v>
+      </c>
+      <c r="F2">
+        <v>297</v>
+      </c>
+      <c r="G2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>78</v>
+      </c>
+      <c r="B3">
+        <v>219</v>
+      </c>
+      <c r="C3">
+        <v>406</v>
+      </c>
+      <c r="D3">
+        <v>641</v>
+      </c>
+      <c r="E3">
+        <v>281</v>
+      </c>
+      <c r="F3">
+        <v>203</v>
+      </c>
+      <c r="G3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>141</v>
+      </c>
+      <c r="B4">
+        <v>203</v>
+      </c>
+      <c r="C4">
+        <v>641</v>
+      </c>
+      <c r="D4">
+        <v>812</v>
+      </c>
+      <c r="E4">
+        <v>344</v>
+      </c>
+      <c r="F4">
+        <v>250</v>
+      </c>
+      <c r="G4">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>78</v>
+      </c>
+      <c r="B5">
+        <v>188</v>
+      </c>
+      <c r="C5">
+        <v>594</v>
+      </c>
+      <c r="D5">
+        <v>937</v>
+      </c>
+      <c r="E5">
+        <v>313</v>
+      </c>
+      <c r="F5">
+        <v>203</v>
+      </c>
+      <c r="G5">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>93</v>
+      </c>
+      <c r="B6">
+        <v>203</v>
+      </c>
+      <c r="C6">
+        <v>704</v>
+      </c>
+      <c r="D6">
+        <v>500</v>
+      </c>
+      <c r="E6">
+        <v>281</v>
+      </c>
+      <c r="F6">
+        <v>187</v>
+      </c>
+      <c r="G6">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>110</v>
+      </c>
+      <c r="B7">
+        <v>234</v>
+      </c>
+      <c r="C7">
+        <v>844</v>
+      </c>
+      <c r="D7">
+        <v>734</v>
+      </c>
+      <c r="E7">
+        <v>282</v>
+      </c>
+      <c r="F7">
+        <v>218</v>
+      </c>
+      <c r="G7">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>93</v>
+      </c>
+      <c r="B8">
+        <v>188</v>
+      </c>
+      <c r="C8">
+        <v>578</v>
+      </c>
+      <c r="D8">
+        <v>328</v>
+      </c>
+      <c r="E8">
+        <v>266</v>
+      </c>
+      <c r="F8">
+        <v>219</v>
+      </c>
+      <c r="G8">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>78</v>
+      </c>
+      <c r="B9">
+        <v>203</v>
+      </c>
+      <c r="C9">
+        <v>532</v>
+      </c>
+      <c r="D9">
+        <v>546</v>
+      </c>
+      <c r="E9">
+        <v>360</v>
+      </c>
+      <c r="F9">
+        <v>172</v>
+      </c>
+      <c r="G9">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>172</v>
+      </c>
+      <c r="B10">
+        <v>172</v>
+      </c>
+      <c r="C10">
+        <v>422</v>
+      </c>
+      <c r="D10">
+        <v>344</v>
+      </c>
+      <c r="E10">
+        <v>296</v>
+      </c>
+      <c r="F10">
+        <v>172</v>
+      </c>
+      <c r="G10">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f>AVERAGE(A1:A10)</f>
+        <v>103.1</v>
+      </c>
+      <c r="B12">
+        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <v>201.6</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>633</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>581.1</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>306.39999999999998</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>215.5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>228</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Populating the impostor scores now.
</commit_message>
<xml_diff>
--- a/QUML_Keystrokes/MD_Double_Check.xlsx
+++ b/QUML_Keystrokes/MD_Double_Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="9"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="User 1" sheetId="1" r:id="rId1"/>
@@ -724,10 +724,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,6 +990,306 @@
       <c r="G12">
         <f t="shared" si="0"/>
         <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f>ABS(A1-A12)/10</f>
+        <v>0.15</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:G14" si="1">ABS(B1-B12)/10</f>
+        <v>3.05</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>7.94</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>6.8899999999999979</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1.2600000000000022</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>7.0300000000000011</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f>ABS(A2-A12)/10</f>
+        <v>0.15</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:G15" si="2">ABS(B2-B12)/10</f>
+        <v>1.55</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>1.3599999999999994</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>15.010000000000002</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0.33999999999999775</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>7.0300000000000011</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>ABS(A3-A12)/10</f>
+        <v>3.25</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:G16" si="3">ABS(B3-B12)/10</f>
+        <v>3.15</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>7.94</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>5.2899999999999974</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>4.3600000000000021</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>0.76999999999999891</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f>ABS(A4-A12)/10</f>
+        <v>0.15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:G17" si="4">ABS(B4-B12)/10</f>
+        <v>1.55</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="4"/>
+        <v>7.6599999999999993</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>4.1100000000000021</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>5.0399999999999974</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>2.2699999999999987</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f>ABS(A5-A12)/10</f>
+        <v>3.05</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ref="B18:G18" si="5">ABS(B5-B12)/10</f>
+        <v>0.05</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="5"/>
+        <v>3.2400000000000007</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="5"/>
+        <v>0.58999999999999775</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="5"/>
+        <v>0.33999999999999775</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>0.83000000000000118</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f>ABS(A6-A12)/10</f>
+        <v>1.35</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:G19" si="6">ABS(B6-B12)/10</f>
+        <v>0.05</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="6"/>
+        <v>6.06</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="6"/>
+        <v>3.7899999999999978</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>3.4399999999999977</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>5.4699999999999989</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="6"/>
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f>ABS(A7-A12)/10</f>
+        <v>0.15</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:G20" si="7">ABS(B7-B12)/10</f>
+        <v>1.55</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="7"/>
+        <v>6.06</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="7"/>
+        <v>0.68999999999999773</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>10.660000000000002</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>5.4300000000000015</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f>ABS(A8-A12)/10</f>
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:G21" si="8">ABS(B8-B12)/10</f>
+        <v>3.15</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="8"/>
+        <v>7.6599999999999993</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="8"/>
+        <v>10.310000000000002</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="8"/>
+        <v>2.8600000000000021</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>0.86999999999999889</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="8"/>
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>ABS(A9-A12)/10</f>
+        <v>2.95</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:G22" si="9">ABS(B9-B12)/10</f>
+        <v>0.05</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="9"/>
+        <v>1.3599999999999994</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="9"/>
+        <v>6.8899999999999979</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="9"/>
+        <v>0.33999999999999775</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="9"/>
+        <v>6.9699999999999989</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="9"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f>ABS(A10-A12)/10</f>
+        <v>1.35</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:G23" si="10">ABS(B10-B12)/10</f>
+        <v>1.55</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="10"/>
+        <v>11.040000000000001</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="10"/>
+        <v>5.2899999999999974</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="10"/>
+        <v>9.639999999999997</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="10"/>
+        <v>3.9699999999999989</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="10"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12:G12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Latest code and calculating the standard deviation
</commit_message>
<xml_diff>
--- a/QUML_Keystrokes/MD_Double_Check.xlsx
+++ b/QUML_Keystrokes/MD_Double_Check.xlsx
@@ -20,6 +20,14 @@
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+  <si>
+    <t>Mean</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -53,8 +61,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="A23" sqref="A23:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>156</v>
       </c>
@@ -390,7 +402,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>172</v>
       </c>
@@ -413,7 +425,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>157</v>
       </c>
@@ -436,7 +448,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>172</v>
       </c>
@@ -459,7 +471,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>187</v>
       </c>
@@ -482,7 +494,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>188</v>
       </c>
@@ -505,7 +517,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>203</v>
       </c>
@@ -528,7 +540,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>172</v>
       </c>
@@ -551,7 +563,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>172</v>
       </c>
@@ -574,7 +586,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>172</v>
       </c>
@@ -597,7 +609,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>AVERAGE(A1:A10)</f>
         <v>175.1</v>
@@ -626,8 +638,12 @@
         <f t="shared" si="0"/>
         <v>201.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>ABS(A1-A12)/10</f>
         <v>1.9099999999999995</v>
@@ -657,7 +673,7 @@
         <v>0.14000000000000057</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>ABS(A2-A12)/10</f>
         <v>0.30999999999999944</v>
@@ -687,7 +703,7 @@
         <v>3.3400000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>ABS(A3-A12)/10</f>
         <v>1.8099999999999994</v>
@@ -717,7 +733,220 @@
         <v>1.6400000000000006</v>
       </c>
     </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f>ABS(A4-A12)/10</f>
+        <v>0.30999999999999944</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:G17" si="4">ABS(B4-B12)/10</f>
+        <v>1.5900000000000005</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="4"/>
+        <v>9.4300000000000015</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>1.0800000000000012</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>4.9899999999999975</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>2.8099999999999996</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>1.3599999999999994</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f>ABS(A5-A12)/10</f>
+        <v>1.1900000000000006</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ref="B18:G18" si="5">ABS(B5-B12)/10</f>
+        <v>9.9999999999994312E-3</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="5"/>
+        <v>10.969999999999999</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="5"/>
+        <v>4.2800000000000011</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="5"/>
+        <v>2.7100000000000022</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>0.29000000000000059</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>3.2400000000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f>ABS(A6-A12)/10</f>
+        <v>1.2900000000000005</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:G19" si="6">ABS(B6-B12)/10</f>
+        <v>3.1099999999999994</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="6"/>
+        <v>9.3300000000000018</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="6"/>
+        <v>15.180000000000001</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>1.2100000000000022</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>2.9099999999999993</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="6"/>
+        <v>1.3599999999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f>ABS(A7-A12)/10</f>
+        <v>2.7900000000000005</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:G20" si="7">ABS(B7-B12)/10</f>
+        <v>9.9999999999994312E-3</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="7"/>
+        <v>7.830000000000001</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="7"/>
+        <v>25.52</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>0.2899999999999977</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>0.29000000000000059</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>3.3400000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f>ABS(A8-A12)/10</f>
+        <v>0.30999999999999944</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:G21" si="8">ABS(B8-B12)/10</f>
+        <v>3.0900000000000007</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="8"/>
+        <v>10.87</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="8"/>
+        <v>7.2800000000000011</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="8"/>
+        <v>6.0100000000000025</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>3.4900000000000007</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="8"/>
+        <v>2.9599999999999995</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>ABS(A9-A12)/10</f>
+        <v>0.30999999999999944</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:G22" si="9">ABS(B9-B12)/10</f>
+        <v>6.2900000000000009</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="9"/>
+        <v>4.6300000000000008</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="9"/>
+        <v>17.619999999999997</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="9"/>
+        <v>9.6899999999999977</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="9"/>
+        <v>1.2099999999999995</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="9"/>
+        <v>3.2400000000000007</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f>ABS(A10-A12)/10</f>
+        <v>0.30999999999999944</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:G23" si="10">ABS(B10-B12)/10</f>
+        <v>1.5900000000000005</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="10"/>
+        <v>4.7300000000000013</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="10"/>
+        <v>20.82</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="10"/>
+        <v>2.8100000000000023</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="10"/>
+        <v>1.8900000000000006</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="10"/>
+        <v>9.26</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H12:I12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1299,15 +1528,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:G12"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>187</v>
       </c>
@@ -1329,8 +1558,12 @@
       <c r="G1">
         <v>313</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="K1">
+        <f>_xlfn.STDEV.S(A1:A10)</f>
+        <v>29.396900819266225</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>234</v>
       </c>
@@ -1353,7 +1586,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>188</v>
       </c>
@@ -1376,7 +1609,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>156</v>
       </c>
@@ -1399,7 +1632,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>140</v>
       </c>
@@ -1422,7 +1655,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>156</v>
       </c>
@@ -1445,7 +1678,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>141</v>
       </c>
@@ -1468,7 +1701,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>157</v>
       </c>
@@ -1491,7 +1724,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>172</v>
       </c>
@@ -1514,7 +1747,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>141</v>
       </c>
@@ -1537,7 +1770,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>AVERAGE(A1:A10)</f>
         <v>167.2</v>
@@ -1566,8 +1799,319 @@
         <f t="shared" si="0"/>
         <v>242.3</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f>ABS(A1-A12)/10</f>
+        <v>1.9800000000000011</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:G14" si="1">ABS(B1-B12)/10</f>
+        <v>1.05</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>2.6599999999999993</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>19.22</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>6.080000000000001</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>7.0600000000000023</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>7.0699999999999985</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f>ABS(A2-A12)/10</f>
+        <v>6.6800000000000015</v>
+      </c>
+      <c r="B15">
+        <f t="shared" ref="B15:G15" si="2">ABS(B2-B12)/10</f>
+        <v>1.05</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="2"/>
+        <v>3.6400000000000006</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>1.0800000000000012</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>4.580000000000001</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="2"/>
+        <v>7.0600000000000023</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>3.8699999999999988</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f>ABS(A3-A12)/10</f>
+        <v>2.080000000000001</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:G16" si="3">ABS(B3-B12)/10</f>
+        <v>2.65</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="3"/>
+        <v>3.6400000000000006</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="3"/>
+        <v>5.7800000000000011</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>3.2199999999999989</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>21.04</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>8.5300000000000011</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f>ABS(A4-A12)/10</f>
+        <v>1.1199999999999988</v>
+      </c>
+      <c r="B17">
+        <f t="shared" ref="B17:G17" si="4">ABS(B4-B12)/10</f>
+        <v>2.65</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="4"/>
+        <v>2.0400000000000005</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="4"/>
+        <v>2.0199999999999987</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
+        <v>1.7199999999999989</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="4"/>
+        <v>2.2600000000000025</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="4"/>
+        <v>6.9699999999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f>ABS(A5-A12)/10</f>
+        <v>2.7199999999999989</v>
+      </c>
+      <c r="B18">
+        <f t="shared" ref="B18:G18" si="5">ABS(B5-B12)/10</f>
+        <v>1.05</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="5"/>
+        <v>8.86</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="5"/>
+        <v>1.0800000000000012</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="5"/>
+        <v>6.419999999999999</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="5"/>
+        <v>3.8600000000000021</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>2.330000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f>ABS(A6-A12)/10</f>
+        <v>1.1199999999999988</v>
+      </c>
+      <c r="B19">
+        <f t="shared" ref="B19:G19" si="6">ABS(B6-B12)/10</f>
+        <v>17.649999999999999</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="6"/>
+        <v>5.76</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="6"/>
+        <v>8.8800000000000008</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="6"/>
+        <v>1.7199999999999989</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>0.73999999999999777</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="6"/>
+        <v>0.76999999999999891</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f>ABS(A7-A12)/10</f>
+        <v>2.6199999999999988</v>
+      </c>
+      <c r="B20">
+        <f t="shared" ref="B20:G20" si="7">ABS(B7-B12)/10</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="7"/>
+        <v>2.6599999999999993</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="7"/>
+        <v>8.3199999999999985</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="7"/>
+        <v>9.1800000000000015</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="7"/>
+        <v>2.3399999999999976</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="7"/>
+        <v>0.73000000000000109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f>ABS(A8-A12)/10</f>
+        <v>1.0199999999999989</v>
+      </c>
+      <c r="B21">
+        <f t="shared" ref="B21:G21" si="8">ABS(B8-B12)/10</f>
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="8"/>
+        <v>3.5400000000000005</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="8"/>
+        <v>7.3800000000000008</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="8"/>
+        <v>1.7199999999999989</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="8"/>
+        <v>0.76000000000000223</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="8"/>
+        <v>3.930000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f>ABS(A9-A12)/10</f>
+        <v>0.48000000000000115</v>
+      </c>
+      <c r="B22">
+        <f t="shared" ref="B22:G22" si="9">ABS(B9-B12)/10</f>
+        <v>2.65</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="9"/>
+        <v>3.5400000000000005</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="9"/>
+        <v>7.3800000000000008</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="9"/>
+        <v>1.7199999999999989</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="9"/>
+        <v>0.76000000000000223</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="9"/>
+        <v>0.83000000000000118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f>ABS(A10-A12)/10</f>
+        <v>2.6199999999999988</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:G23" si="10">ABS(B10-B12)/10</f>
+        <v>4.25</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="10"/>
+        <v>3.5400000000000005</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="10"/>
+        <v>2.0199999999999987</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="10"/>
+        <v>3.319999999999999</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="10"/>
+        <v>2.3600000000000021</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="10"/>
+        <v>2.330000000000001</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H12:I12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Making some double checking changes with the Excel file to double check everything
</commit_message>
<xml_diff>
--- a/QUML_Keystrokes/MD_Double_Check.xlsx
+++ b/QUML_Keystrokes/MD_Double_Check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="User 1" sheetId="1" r:id="rId1"/>
@@ -371,15 +371,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>156</v>
       </c>
@@ -401,8 +401,12 @@
       <c r="G1">
         <v>203</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1">
+        <f>STDEV(A1:A10)</f>
+        <v>14.247416919880211</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>172</v>
       </c>
@@ -424,8 +428,12 @@
       <c r="G2">
         <v>235</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J2">
+        <f t="shared" ref="J2:J10" si="0">STDEV(A2:A11)</f>
+        <v>13.330207967036538</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>157</v>
       </c>
@@ -447,8 +455,12 @@
       <c r="G3">
         <v>218</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>13.217980178529546</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>172</v>
       </c>
@@ -470,8 +482,12 @@
       <c r="G4">
         <v>188</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>11.475805293871849</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>187</v>
       </c>
@@ -493,8 +509,12 @@
       <c r="G5">
         <v>234</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>64.369863831166043</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>188</v>
       </c>
@@ -516,8 +536,12 @@
       <c r="G6">
         <v>188</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>83.666020923328603</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>203</v>
       </c>
@@ -539,8 +563,12 @@
       <c r="G7">
         <v>235</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>92.426297423174674</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>172</v>
       </c>
@@ -562,8 +590,12 @@
       <c r="G8">
         <v>172</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>91.779648537757481</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>172</v>
       </c>
@@ -585,8 +617,12 @@
       <c r="G9">
         <v>234</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>88.987930873076436</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>172</v>
       </c>
@@ -608,34 +644,38 @@
       <c r="G10">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>79.818352526220437</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>AVERAGE(A1:A10)</f>
         <v>175.1</v>
       </c>
       <c r="B12">
-        <f t="shared" ref="B12:G12" si="0">AVERAGE(B1:B10)</f>
+        <f t="shared" ref="B12:G12" si="1">AVERAGE(B1:B10)</f>
         <v>171.9</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>234.3</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>479.8</v>
       </c>
       <c r="E12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>356.1</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>200.1</v>
       </c>
       <c r="G12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>201.6</v>
       </c>
       <c r="H12" s="2" t="s">
@@ -643,93 +683,93 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>ABS(A1-A12)/10</f>
         <v>1.9099999999999995</v>
       </c>
       <c r="B14">
-        <f t="shared" ref="B14:G14" si="1">ABS(B1-B12)/10</f>
+        <f t="shared" ref="B14:G14" si="2">ABS(B1-B12)/10</f>
         <v>1.6099999999999994</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.169999999999999</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.48</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.3100000000000023</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.8900000000000006</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.14000000000000057</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>ABS(A2-A12)/10</f>
         <v>0.30999999999999944</v>
       </c>
       <c r="B15">
-        <f t="shared" ref="B15:G15" si="2">ABS(B2-B12)/10</f>
+        <f t="shared" ref="B15:G15" si="3">ABS(B2-B12)/10</f>
         <v>6.31</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.7699999999999987</v>
       </c>
       <c r="D15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8.8800000000000008</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.2899999999999977</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.29000000000000059</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.3400000000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>ABS(A3-A12)/10</f>
         <v>1.8099999999999994</v>
       </c>
       <c r="B16">
-        <f t="shared" ref="B16:G16" si="3">ABS(B3-B12)/10</f>
+        <f t="shared" ref="B16:G16" si="4">ABS(B3-B12)/10</f>
         <v>1.5099999999999993</v>
       </c>
       <c r="C16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.169999999999999</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.78</v>
       </c>
       <c r="E16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2100000000000022</v>
       </c>
       <c r="F16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.2099999999999995</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.6400000000000006</v>
       </c>
     </row>
@@ -739,27 +779,27 @@
         <v>0.30999999999999944</v>
       </c>
       <c r="B17">
-        <f t="shared" ref="B17:G17" si="4">ABS(B4-B12)/10</f>
+        <f t="shared" ref="B17:G17" si="5">ABS(B4-B12)/10</f>
         <v>1.5900000000000005</v>
       </c>
       <c r="C17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.4300000000000015</v>
       </c>
       <c r="D17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0800000000000012</v>
       </c>
       <c r="E17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.9899999999999975</v>
       </c>
       <c r="F17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8099999999999996</v>
       </c>
       <c r="G17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3599999999999994</v>
       </c>
     </row>
@@ -769,27 +809,27 @@
         <v>1.1900000000000006</v>
       </c>
       <c r="B18">
-        <f t="shared" ref="B18:G18" si="5">ABS(B5-B12)/10</f>
+        <f t="shared" ref="B18:G18" si="6">ABS(B5-B12)/10</f>
         <v>9.9999999999994312E-3</v>
       </c>
       <c r="C18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10.969999999999999</v>
       </c>
       <c r="D18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.2800000000000011</v>
       </c>
       <c r="E18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.7100000000000022</v>
       </c>
       <c r="F18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.29000000000000059</v>
       </c>
       <c r="G18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.2400000000000007</v>
       </c>
     </row>
@@ -799,27 +839,27 @@
         <v>1.2900000000000005</v>
       </c>
       <c r="B19">
-        <f t="shared" ref="B19:G19" si="6">ABS(B6-B12)/10</f>
+        <f t="shared" ref="B19:G19" si="7">ABS(B6-B12)/10</f>
         <v>3.1099999999999994</v>
       </c>
       <c r="C19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>9.3300000000000018</v>
       </c>
       <c r="D19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>15.180000000000001</v>
       </c>
       <c r="E19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.2100000000000022</v>
       </c>
       <c r="F19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.9099999999999993</v>
       </c>
       <c r="G19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1.3599999999999994</v>
       </c>
     </row>
@@ -829,27 +869,27 @@
         <v>2.7900000000000005</v>
       </c>
       <c r="B20">
-        <f t="shared" ref="B20:G20" si="7">ABS(B7-B12)/10</f>
+        <f t="shared" ref="B20:G20" si="8">ABS(B7-B12)/10</f>
         <v>9.9999999999994312E-3</v>
       </c>
       <c r="C20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>7.830000000000001</v>
       </c>
       <c r="D20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>25.52</v>
       </c>
       <c r="E20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.2899999999999977</v>
       </c>
       <c r="F20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.29000000000000059</v>
       </c>
       <c r="G20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>3.3400000000000007</v>
       </c>
     </row>
@@ -859,27 +899,27 @@
         <v>0.30999999999999944</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:G21" si="8">ABS(B8-B12)/10</f>
+        <f t="shared" ref="B21:G21" si="9">ABS(B8-B12)/10</f>
         <v>3.0900000000000007</v>
       </c>
       <c r="C21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>10.87</v>
       </c>
       <c r="D21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>7.2800000000000011</v>
       </c>
       <c r="E21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>6.0100000000000025</v>
       </c>
       <c r="F21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>3.4900000000000007</v>
       </c>
       <c r="G21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>2.9599999999999995</v>
       </c>
     </row>
@@ -889,27 +929,27 @@
         <v>0.30999999999999944</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:G22" si="9">ABS(B9-B12)/10</f>
+        <f t="shared" ref="B22:G22" si="10">ABS(B9-B12)/10</f>
         <v>6.2900000000000009</v>
       </c>
       <c r="C22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>4.6300000000000008</v>
       </c>
       <c r="D22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>17.619999999999997</v>
       </c>
       <c r="E22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>9.6899999999999977</v>
       </c>
       <c r="F22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1.2099999999999995</v>
       </c>
       <c r="G22">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>3.2400000000000007</v>
       </c>
     </row>
@@ -919,27 +959,27 @@
         <v>0.30999999999999944</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:G23" si="10">ABS(B10-B12)/10</f>
+        <f t="shared" ref="B23:G23" si="11">ABS(B10-B12)/10</f>
         <v>1.5900000000000005</v>
       </c>
       <c r="C23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>4.7300000000000013</v>
       </c>
       <c r="D23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>20.82</v>
       </c>
       <c r="E23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>2.8100000000000023</v>
       </c>
       <c r="F23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.8900000000000006</v>
       </c>
       <c r="G23">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>9.26</v>
       </c>
     </row>
@@ -1530,7 +1570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>

</xml_diff>